<commit_message>
Added documentation and few fixes
</commit_message>
<xml_diff>
--- a/documentation/DatabaseModel.xlsx
+++ b/documentation/DatabaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BITSProject\CPADAssignment-1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473EF497-5A2F-4B84-8212-B2F2A54DFC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B30374-3F26-4F1A-8BE4-6ED8D34C85A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{7569AB63-CD0F-407D-A1C1-8FB414BFCF75}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{7569AB63-CD0F-407D-A1C1-8FB414BFCF75}"/>
   </bookViews>
   <sheets>
     <sheet name="StudentVaccinationDetails" sheetId="2" r:id="rId1"/>
@@ -112,12 +112,6 @@
 vaccines</t>
   </si>
   <si>
-    <t>[{"doseNo":1,"date":1122020,"name":"Covaxine","batchNo":"111222"},{"doseNo":2,"date":1122021,"name":"Covaxine","batchNo":"333222"}]</t>
-  </si>
-  <si>
-    <t>for reporting , derived from 'doseDetails'</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vaccinated or not </t>
   </si>
   <si>
@@ -220,6 +214,14 @@
   </si>
   <si>
     <t>https://parsefiles.back4app.com/pNWxjrix1cu6IokwslWDmklCfdl6X8obnLnTp9bY/acb64186be43a9283fd192919a9ce23d_sample.csv_14102022</t>
+  </si>
+  <si>
+    <t>[{"doseNo":1,"date":1122020,"name":"Covaxine","batchNo":"111222"}
+,{"doseNo":2,"date":1122021,"name":"Covaxine","batchNo":"333222"}]</t>
+  </si>
+  <si>
+    <t>for reporting , derived
+ from 'doseDetails'</t>
   </si>
 </sst>
 </file>
@@ -321,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -329,13 +331,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,22 +658,22 @@
   <dimension ref="C2:E16"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C2" sqref="C2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
@@ -733,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -744,16 +749,16 @@
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="E10" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -762,43 +767,43 @@
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="3:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="3:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -815,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586264FB-D1BB-46B9-BEA4-9A92A30E1ADB}">
   <dimension ref="D2:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,11 +832,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D3" s="2" t="s">
@@ -855,21 +860,21 @@
     </row>
     <row r="5" spans="4:6" ht="29" x14ac:dyDescent="0.35">
       <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -878,10 +883,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="4:6" x14ac:dyDescent="0.35">
@@ -889,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -897,28 +902,28 @@
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>44</v>
+      <c r="E9" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>32</v>
+      <c r="D11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -934,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FCC1D7-1146-4E77-9D32-EE3BFD575AA2}">
   <dimension ref="E2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -946,11 +951,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:7" x14ac:dyDescent="0.35">
-      <c r="E2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E3" s="2" t="s">
@@ -974,39 +979,39 @@
     </row>
     <row r="5" spans="5:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="5:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
@@ -1014,30 +1019,30 @@
     </row>
     <row r="9" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1"/>
     </row>

</xml_diff>